<commit_message>
[UPDATE] UPDATE budget, kurs, realization
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Tempalate Fix.xlsx
+++ b/uploads/excel/RKAP Tempalate Fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF76EE1-8BB0-4F6D-A004-D9A6CBE974D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580BA9F9-C7C6-4503-B5FC-93910E8EF537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="td2023" sheetId="1" r:id="rId1"/>
@@ -1672,7 +1672,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Year</t>
   </si>
@@ -1721,12 +1721,30 @@
   <si>
     <t>ZGMFTA</t>
   </si>
+  <si>
+    <t>MATERIAL EXPENSES</t>
+  </si>
+  <si>
+    <t>SUBCONTRACT EXPENSES</t>
+  </si>
+  <si>
+    <t>financialIndicator</t>
+  </si>
+  <si>
+    <t>subFinancialIndicator</t>
+  </si>
+  <si>
+    <t>Rotable parts-Subcont</t>
+  </si>
+  <si>
+    <t>Expendable-Material</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1738,6 +1756,10 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1757,8 +1779,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1775,8 +1798,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{9BB36901-0947-482B-96B9-193C962DAE43}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1992,15 +2016,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2008,63 +2036,69 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>2023</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4">
         <v>40011110</v>
       </c>
-      <c r="D2" s="3">
+      <c r="F2" s="3">
         <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1200</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1200</v>
       </c>
       <c r="G2" s="3">
         <v>1200</v>
@@ -2093,23 +2127,29 @@
       <c r="O2" s="3">
         <v>1200</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="3">
+        <v>1200</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1">
       <c r="A3" s="4">
         <v>2023</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4">
         <v>40011120</v>
       </c>
-      <c r="D3" s="3">
-        <v>132</v>
-      </c>
-      <c r="E3" s="3">
-        <v>132</v>
-      </c>
       <c r="F3" s="3">
         <v>132</v>
       </c>
@@ -2140,32 +2180,38 @@
       <c r="O3" s="3">
         <v>132</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="3">
+        <v>132</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>2023</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4">
         <v>40011130</v>
       </c>
-      <c r="D4" s="3">
-        <v>132</v>
-      </c>
-      <c r="E4" s="3">
-        <v>132</v>
-      </c>
       <c r="F4" s="3">
+        <v>132</v>
+      </c>
+      <c r="G4" s="3">
+        <v>132</v>
+      </c>
+      <c r="H4" s="3">
         <v>110</v>
       </c>
-      <c r="G4" s="3">
-        <v>132</v>
-      </c>
-      <c r="H4" s="3">
-        <v>132</v>
-      </c>
       <c r="I4" s="3">
         <v>132</v>
       </c>
@@ -2187,47 +2233,125 @@
       <c r="O4" s="3">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P4" s="3">
+        <v>132</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A5" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4">
+        <v>40020010</v>
+      </c>
+      <c r="F5" s="3">
+        <v>132</v>
+      </c>
+      <c r="G5" s="3">
+        <v>132</v>
+      </c>
+      <c r="H5" s="3">
+        <v>110</v>
+      </c>
+      <c r="I5" s="3">
+        <v>132</v>
+      </c>
+      <c r="J5" s="3">
+        <v>132</v>
+      </c>
+      <c r="K5" s="3">
+        <v>132</v>
+      </c>
+      <c r="L5" s="3">
+        <v>132</v>
+      </c>
+      <c r="M5" s="3">
+        <v>132</v>
+      </c>
+      <c r="N5" s="3">
+        <v>132</v>
+      </c>
+      <c r="O5" s="3">
+        <v>132</v>
+      </c>
+      <c r="P5" s="3">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A6" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4">
+        <v>40020011</v>
+      </c>
+      <c r="F6" s="3">
+        <v>150</v>
+      </c>
+      <c r="G6" s="3">
+        <v>150</v>
+      </c>
+      <c r="H6" s="3">
+        <v>150</v>
+      </c>
+      <c r="I6" s="3">
+        <v>150</v>
+      </c>
+      <c r="J6" s="3">
+        <v>150</v>
+      </c>
+      <c r="K6" s="3">
+        <v>150</v>
+      </c>
+      <c r="L6" s="3">
+        <v>150</v>
+      </c>
+      <c r="M6" s="3">
+        <v>150</v>
+      </c>
+      <c r="N6" s="3">
+        <v>150</v>
+      </c>
+      <c r="O6" s="3">
+        <v>150</v>
+      </c>
+      <c r="P6" s="3">
+        <v>150</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2238,13 +2362,15 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2255,13 +2381,15 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2272,13 +2400,15 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2289,13 +2419,15 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2306,13 +2438,15 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2323,13 +2457,15 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2340,13 +2476,15 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2357,13 +2495,15 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2374,13 +2514,15 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2391,13 +2533,15 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2408,13 +2552,15 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -2425,13 +2571,15 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2442,13 +2590,15 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2459,13 +2609,15 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2476,13 +2628,15 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2493,13 +2647,15 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2510,13 +2666,15 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2527,13 +2685,15 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2544,13 +2704,15 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -2561,13 +2723,15 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" customHeight="1">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2578,13 +2742,15 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="4"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -2595,13 +2761,15 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" customHeight="1">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="4"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2612,13 +2780,15 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2629,13 +2799,15 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1">
       <c r="A31" s="4"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2646,13 +2818,15 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" customHeight="1">
       <c r="A32" s="4"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="4"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2663,13 +2837,15 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -2680,13 +2856,15 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" ht="15.75" customHeight="1">
       <c r="A34" s="4"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -2697,13 +2875,15 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" customHeight="1">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -2714,13 +2894,15 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" customHeight="1">
       <c r="A36" s="4"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="4"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2731,13 +2913,15 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" ht="12.75">
       <c r="A37" s="4"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2748,13 +2932,15 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-    </row>
-    <row r="38" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+    </row>
+    <row r="38" spans="1:17" ht="12.75">
       <c r="A38" s="4"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="4"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -2765,13 +2951,15 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17" ht="12.75">
       <c r="A39" s="4"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="4"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -2782,13 +2970,15 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-    </row>
-    <row r="40" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+    </row>
+    <row r="40" spans="1:17" ht="12.75">
       <c r="A40" s="4"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -2799,13 +2989,15 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+    </row>
+    <row r="41" spans="1:17" ht="12.75">
       <c r="A41" s="4"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2816,6 +3008,8 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[UPDATE] Sum dari Variable
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Tempalate Fix.xlsx
+++ b/uploads/excel/RKAP Tempalate Fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA6425A-D00C-4429-AF5B-81E5E7796105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A40AA73-9A18-4E8C-A8CA-156B38C4C82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="td2023" sheetId="1" r:id="rId1"/>
@@ -1683,42 +1683,6 @@
     <t>GlAccount</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>Mei</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Jul</t>
-  </si>
-  <si>
-    <t>Aug</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Nop</t>
-  </si>
-  <si>
-    <t>Des</t>
-  </si>
-  <si>
     <t>ZGMFTA</t>
   </si>
   <si>
@@ -1754,12 +1718,48 @@
   <si>
     <t>Corporate Event</t>
   </si>
+  <si>
+    <t>value01</t>
+  </si>
+  <si>
+    <t>value02</t>
+  </si>
+  <si>
+    <t>value03</t>
+  </si>
+  <si>
+    <t>value04</t>
+  </si>
+  <si>
+    <t>value05</t>
+  </si>
+  <si>
+    <t>value06</t>
+  </si>
+  <si>
+    <t>value07</t>
+  </si>
+  <si>
+    <t>value08</t>
+  </si>
+  <si>
+    <t>value09</t>
+  </si>
+  <si>
+    <t>value10</t>
+  </si>
+  <si>
+    <t>value11</t>
+  </si>
+  <si>
+    <t>value12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1777,6 +1777,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2036,8 +2041,8 @@
   </sheetPr>
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2054,49 +2059,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2104,13 +2109,13 @@
         <v>2023</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4">
         <v>40011110</v>
@@ -2151,7 +2156,10 @@
       <c r="Q2" s="3">
         <v>210</v>
       </c>
-      <c r="R2" s="5"/>
+      <c r="R2" s="5">
+        <f>SUM(F2:Q2)</f>
+        <v>1860</v>
+      </c>
       <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2159,19 +2167,19 @@
         <v>2023</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4">
         <v>40011120</v>
       </c>
       <c r="F3" s="3">
-        <v>110</v>
+        <v>-110</v>
       </c>
       <c r="G3" s="3">
         <v>120</v>
@@ -2213,13 +2221,13 @@
         <v>2023</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4">
         <v>40011130</v>
@@ -2267,13 +2275,13 @@
         <v>2023</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4">
         <v>40013001</v>
@@ -2320,13 +2328,13 @@
         <v>2023</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4">
         <v>40013002</v>
@@ -2373,13 +2381,13 @@
         <v>2023</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4">
         <v>40013003</v>
@@ -2426,13 +2434,13 @@
         <v>2023</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4">
         <v>40013010</v>
@@ -2479,13 +2487,13 @@
         <v>2023</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4">
         <v>40013015</v>
@@ -2532,13 +2540,13 @@
         <v>2023</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4">
         <v>40013016</v>
@@ -2585,13 +2593,13 @@
         <v>2023</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4">
         <v>40013017</v>
@@ -2638,13 +2646,13 @@
         <v>2023</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E12" s="4">
         <v>40013018</v>
@@ -2691,13 +2699,13 @@
         <v>2023</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E13" s="4">
         <v>40013019</v>
@@ -2744,13 +2752,13 @@
         <v>2023</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4">
         <v>40020010</v>
@@ -2797,13 +2805,13 @@
         <v>2023</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4">
         <v>40020011</v>
@@ -2850,13 +2858,13 @@
         <v>2023</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E16" s="4">
         <v>40043000</v>
@@ -2903,13 +2911,13 @@
         <v>2023</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E17" s="4">
         <v>40043001</v>
@@ -2956,13 +2964,13 @@
         <v>2023</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4">
         <v>40043002</v>
@@ -3009,13 +3017,13 @@
         <v>2023</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E19" s="4">
         <v>40043006</v>
@@ -3062,13 +3070,13 @@
         <v>2023</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E20" s="4">
         <v>40043007</v>
@@ -3115,13 +3123,13 @@
         <v>2023</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E21" s="4">
         <v>40043011</v>
@@ -3563,6 +3571,7 @@
       <c r="Q42" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[UPDATE] Kurs, Return, Budget, Seed
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Tempalate Fix.xlsx
+++ b/uploads/excel/RKAP Tempalate Fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0F050E-F47B-4837-BCFE-30BAFD0482EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8D9E58-9E47-4152-8037-7A00DF032EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="td2023" sheetId="1" r:id="rId1"/>
@@ -1672,7 +1672,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Year</t>
   </si>
@@ -1775,7 +1775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1790,6 +1790,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,7 +2018,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2081,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="4">
-        <v>40011110</v>
+        <v>40010001</v>
       </c>
       <c r="D2" s="3">
         <v>100</v>
@@ -2114,7 +2120,7 @@
         <v>210</v>
       </c>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2124,7 +2130,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>40013001</v>
+        <v>40012000</v>
       </c>
       <c r="D3" s="3">
         <v>-110</v>
@@ -2163,6 +2169,7 @@
         <v>220</v>
       </c>
       <c r="P3" s="5"/>
+      <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -2172,7 +2179,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="4">
-        <v>40020010</v>
+        <v>40020001</v>
       </c>
       <c r="D4" s="3">
         <v>120</v>
@@ -2211,6 +2218,7 @@
         <v>230</v>
       </c>
       <c r="P4" s="5"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
@@ -2220,7 +2228,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="4">
-        <v>40043000</v>
+        <v>40014200</v>
       </c>
       <c r="D5" s="3">
         <v>130</v>
@@ -2258,6 +2266,8 @@
       <c r="O5" s="3">
         <v>130</v>
       </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="7"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -2267,7 +2277,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="4">
-        <v>40043006</v>
+        <v>40000000</v>
       </c>
       <c r="D6" s="3">
         <v>140</v>
@@ -2305,6 +2315,8 @@
       <c r="O6" s="3">
         <v>140</v>
       </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
@@ -2314,7 +2326,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="4">
-        <v>40044011</v>
+        <v>40002002</v>
       </c>
       <c r="D7" s="3">
         <v>150</v>
@@ -2352,16 +2364,18 @@
       <c r="O7" s="3">
         <v>150</v>
       </c>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4">
-        <v>40011110</v>
+        <v>40000400</v>
       </c>
       <c r="D8" s="3">
         <v>160</v>
@@ -2399,16 +2413,18 @@
       <c r="O8" s="3">
         <v>160</v>
       </c>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="7"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>2023</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4">
-        <v>40013001</v>
+        <v>40000403</v>
       </c>
       <c r="D9" s="3">
         <v>170</v>
@@ -2446,16 +2462,18 @@
       <c r="O9" s="3">
         <v>170</v>
       </c>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>2023</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4">
-        <v>40020010</v>
+        <v>40030000</v>
       </c>
       <c r="D10" s="3">
         <v>180</v>
@@ -2493,16 +2511,18 @@
       <c r="O10" s="3">
         <v>180</v>
       </c>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>2023</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4">
-        <v>40043000</v>
+        <v>40030001</v>
       </c>
       <c r="D11" s="3">
         <v>190</v>
@@ -2540,16 +2560,18 @@
       <c r="O11" s="3">
         <v>190</v>
       </c>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>2023</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4">
-        <v>40043006</v>
+        <v>40040000</v>
       </c>
       <c r="D12" s="3">
         <v>200</v>
@@ -2587,16 +2609,18 @@
       <c r="O12" s="3">
         <v>200</v>
       </c>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>2023</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4">
-        <v>40044011</v>
+        <v>40040005</v>
       </c>
       <c r="D13" s="3">
         <v>210</v>
@@ -2634,346 +2658,948 @@
       <c r="O13" s="3">
         <v>210</v>
       </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="A14" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4">
+        <v>40041002</v>
+      </c>
+      <c r="D14" s="3">
+        <v>220</v>
+      </c>
+      <c r="E14" s="3">
+        <v>220</v>
+      </c>
+      <c r="F14" s="3">
+        <v>220</v>
+      </c>
+      <c r="G14" s="3">
+        <v>220</v>
+      </c>
+      <c r="H14" s="3">
+        <v>220</v>
+      </c>
+      <c r="I14" s="3">
+        <v>220</v>
+      </c>
+      <c r="J14" s="3">
+        <v>220</v>
+      </c>
+      <c r="K14" s="3">
+        <v>220</v>
+      </c>
+      <c r="L14" s="3">
+        <v>220</v>
+      </c>
+      <c r="M14" s="3">
+        <v>220</v>
+      </c>
+      <c r="N14" s="3">
+        <v>220</v>
+      </c>
+      <c r="O14" s="3">
+        <v>220</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="A15" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4">
+        <v>40041000</v>
+      </c>
+      <c r="D15" s="3">
+        <v>230</v>
+      </c>
+      <c r="E15" s="3">
+        <v>230</v>
+      </c>
+      <c r="F15" s="3">
+        <v>230</v>
+      </c>
+      <c r="G15" s="3">
+        <v>230</v>
+      </c>
+      <c r="H15" s="3">
+        <v>230</v>
+      </c>
+      <c r="I15" s="3">
+        <v>230</v>
+      </c>
+      <c r="J15" s="3">
+        <v>230</v>
+      </c>
+      <c r="K15" s="3">
+        <v>230</v>
+      </c>
+      <c r="L15" s="3">
+        <v>230</v>
+      </c>
+      <c r="M15" s="3">
+        <v>230</v>
+      </c>
+      <c r="N15" s="3">
+        <v>230</v>
+      </c>
+      <c r="O15" s="3">
+        <v>230</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="A16" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4">
+        <v>40043000</v>
+      </c>
+      <c r="D16" s="3">
+        <v>240</v>
+      </c>
+      <c r="E16" s="3">
+        <v>240</v>
+      </c>
+      <c r="F16" s="3">
+        <v>240</v>
+      </c>
+      <c r="G16" s="3">
+        <v>240</v>
+      </c>
+      <c r="H16" s="3">
+        <v>240</v>
+      </c>
+      <c r="I16" s="3">
+        <v>240</v>
+      </c>
+      <c r="J16" s="3">
+        <v>240</v>
+      </c>
+      <c r="K16" s="3">
+        <v>240</v>
+      </c>
+      <c r="L16" s="3">
+        <v>240</v>
+      </c>
+      <c r="M16" s="3">
+        <v>240</v>
+      </c>
+      <c r="N16" s="3">
+        <v>240</v>
+      </c>
+      <c r="O16" s="3">
+        <v>240</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
+      <c r="A17" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>40043006</v>
+      </c>
+      <c r="D17" s="3">
+        <v>250</v>
+      </c>
+      <c r="E17" s="3">
+        <v>250</v>
+      </c>
+      <c r="F17" s="3">
+        <v>250</v>
+      </c>
+      <c r="G17" s="3">
+        <v>250</v>
+      </c>
+      <c r="H17" s="3">
+        <v>250</v>
+      </c>
+      <c r="I17" s="3">
+        <v>250</v>
+      </c>
+      <c r="J17" s="3">
+        <v>250</v>
+      </c>
+      <c r="K17" s="3">
+        <v>250</v>
+      </c>
+      <c r="L17" s="3">
+        <v>250</v>
+      </c>
+      <c r="M17" s="3">
+        <v>250</v>
+      </c>
+      <c r="N17" s="3">
+        <v>250</v>
+      </c>
+      <c r="O17" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="A18" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4">
+        <v>40010001</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3">
+        <v>14</v>
+      </c>
+      <c r="I18" s="3">
+        <v>15</v>
+      </c>
+      <c r="J18" s="3">
+        <v>16</v>
+      </c>
+      <c r="K18" s="3">
+        <v>17</v>
+      </c>
+      <c r="L18" s="3">
+        <v>18</v>
+      </c>
+      <c r="M18" s="3">
+        <v>19</v>
+      </c>
+      <c r="N18" s="3">
+        <v>20</v>
+      </c>
+      <c r="O18" s="3">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="A19" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4">
+        <v>40012000</v>
+      </c>
+      <c r="D19" s="3">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3">
+        <v>12</v>
+      </c>
+      <c r="F19" s="3">
+        <v>13</v>
+      </c>
+      <c r="G19" s="3">
+        <v>14</v>
+      </c>
+      <c r="H19" s="3">
+        <v>15</v>
+      </c>
+      <c r="I19" s="3">
+        <v>16</v>
+      </c>
+      <c r="J19" s="3">
+        <v>17</v>
+      </c>
+      <c r="K19" s="3">
+        <v>18</v>
+      </c>
+      <c r="L19" s="3">
+        <v>19</v>
+      </c>
+      <c r="M19" s="3">
+        <v>20</v>
+      </c>
+      <c r="N19" s="3">
+        <v>21</v>
+      </c>
+      <c r="O19" s="3">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
+      <c r="A20" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4">
+        <v>40020001</v>
+      </c>
+      <c r="D20" s="3">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3">
+        <v>13</v>
+      </c>
+      <c r="F20" s="3">
+        <v>14</v>
+      </c>
+      <c r="G20" s="3">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3">
+        <v>16</v>
+      </c>
+      <c r="I20" s="3">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3">
+        <v>18</v>
+      </c>
+      <c r="K20" s="3">
+        <v>19</v>
+      </c>
+      <c r="L20" s="3">
+        <v>20</v>
+      </c>
+      <c r="M20" s="3">
+        <v>21</v>
+      </c>
+      <c r="N20" s="3">
+        <v>22</v>
+      </c>
+      <c r="O20" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="A21" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="4">
+        <v>40014200</v>
+      </c>
+      <c r="D21" s="3">
+        <v>11</v>
+      </c>
+      <c r="E21" s="3">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3">
+        <v>15</v>
+      </c>
+      <c r="G21" s="3">
+        <v>16</v>
+      </c>
+      <c r="H21" s="3">
+        <v>17</v>
+      </c>
+      <c r="I21" s="3">
+        <v>18</v>
+      </c>
+      <c r="J21" s="3">
+        <v>19</v>
+      </c>
+      <c r="K21" s="3">
+        <v>20</v>
+      </c>
+      <c r="L21" s="3">
+        <v>21</v>
+      </c>
+      <c r="M21" s="3">
+        <v>22</v>
+      </c>
+      <c r="N21" s="3">
+        <v>23</v>
+      </c>
+      <c r="O21" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="A22" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="4">
+        <v>40000000</v>
+      </c>
+      <c r="D22" s="3">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3">
+        <v>16</v>
+      </c>
+      <c r="G22" s="3">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3">
+        <v>18</v>
+      </c>
+      <c r="I22" s="3">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3">
+        <v>20</v>
+      </c>
+      <c r="K22" s="3">
+        <v>21</v>
+      </c>
+      <c r="L22" s="3">
+        <v>22</v>
+      </c>
+      <c r="M22" s="3">
+        <v>23</v>
+      </c>
+      <c r="N22" s="3">
+        <v>24</v>
+      </c>
+      <c r="O22" s="3">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
+      <c r="A23" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4">
+        <v>40002002</v>
+      </c>
+      <c r="D23" s="3">
+        <v>15</v>
+      </c>
+      <c r="E23" s="3">
+        <v>16</v>
+      </c>
+      <c r="F23" s="3">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3">
+        <v>18</v>
+      </c>
+      <c r="H23" s="3">
+        <v>19</v>
+      </c>
+      <c r="I23" s="3">
+        <v>20</v>
+      </c>
+      <c r="J23" s="3">
+        <v>21</v>
+      </c>
+      <c r="K23" s="3">
+        <v>22</v>
+      </c>
+      <c r="L23" s="3">
+        <v>23</v>
+      </c>
+      <c r="M23" s="3">
+        <v>24</v>
+      </c>
+      <c r="N23" s="3">
+        <v>25</v>
+      </c>
+      <c r="O23" s="3">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
+      <c r="A24" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="4">
+        <v>40000400</v>
+      </c>
+      <c r="D24" s="3">
+        <v>16</v>
+      </c>
+      <c r="E24" s="3">
+        <v>17</v>
+      </c>
+      <c r="F24" s="3">
+        <v>18</v>
+      </c>
+      <c r="G24" s="3">
+        <v>19</v>
+      </c>
+      <c r="H24" s="3">
+        <v>20</v>
+      </c>
+      <c r="I24" s="3">
+        <v>21</v>
+      </c>
+      <c r="J24" s="3">
+        <v>22</v>
+      </c>
+      <c r="K24" s="3">
+        <v>23</v>
+      </c>
+      <c r="L24" s="3">
+        <v>24</v>
+      </c>
+      <c r="M24" s="3">
+        <v>25</v>
+      </c>
+      <c r="N24" s="3">
+        <v>26</v>
+      </c>
+      <c r="O24" s="3">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+      <c r="A25" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="4">
+        <v>40000403</v>
+      </c>
+      <c r="D25" s="3">
+        <v>17</v>
+      </c>
+      <c r="E25" s="3">
+        <v>18</v>
+      </c>
+      <c r="F25" s="3">
+        <v>19</v>
+      </c>
+      <c r="G25" s="3">
+        <v>20</v>
+      </c>
+      <c r="H25" s="3">
+        <v>21</v>
+      </c>
+      <c r="I25" s="3">
+        <v>22</v>
+      </c>
+      <c r="J25" s="3">
+        <v>23</v>
+      </c>
+      <c r="K25" s="3">
+        <v>24</v>
+      </c>
+      <c r="L25" s="3">
+        <v>25</v>
+      </c>
+      <c r="M25" s="3">
+        <v>26</v>
+      </c>
+      <c r="N25" s="3">
+        <v>27</v>
+      </c>
+      <c r="O25" s="3">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
+      <c r="A26" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="4">
+        <v>40030000</v>
+      </c>
+      <c r="D26" s="3">
+        <v>18</v>
+      </c>
+      <c r="E26" s="3">
+        <v>19</v>
+      </c>
+      <c r="F26" s="3">
+        <v>20</v>
+      </c>
+      <c r="G26" s="3">
+        <v>21</v>
+      </c>
+      <c r="H26" s="3">
+        <v>22</v>
+      </c>
+      <c r="I26" s="3">
+        <v>23</v>
+      </c>
+      <c r="J26" s="3">
+        <v>24</v>
+      </c>
+      <c r="K26" s="3">
+        <v>25</v>
+      </c>
+      <c r="L26" s="3">
+        <v>26</v>
+      </c>
+      <c r="M26" s="3">
+        <v>27</v>
+      </c>
+      <c r="N26" s="3">
+        <v>28</v>
+      </c>
+      <c r="O26" s="3">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
+      <c r="A27" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="4">
+        <v>40030001</v>
+      </c>
+      <c r="D27" s="3">
+        <v>19</v>
+      </c>
+      <c r="E27" s="3">
+        <v>20</v>
+      </c>
+      <c r="F27" s="3">
+        <v>21</v>
+      </c>
+      <c r="G27" s="3">
+        <v>22</v>
+      </c>
+      <c r="H27" s="3">
+        <v>23</v>
+      </c>
+      <c r="I27" s="3">
+        <v>24</v>
+      </c>
+      <c r="J27" s="3">
+        <v>25</v>
+      </c>
+      <c r="K27" s="3">
+        <v>26</v>
+      </c>
+      <c r="L27" s="3">
+        <v>27</v>
+      </c>
+      <c r="M27" s="3">
+        <v>28</v>
+      </c>
+      <c r="N27" s="3">
+        <v>29</v>
+      </c>
+      <c r="O27" s="3">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
+      <c r="A28" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="4">
+        <v>40040000</v>
+      </c>
+      <c r="D28" s="3">
+        <v>20</v>
+      </c>
+      <c r="E28" s="3">
+        <v>21</v>
+      </c>
+      <c r="F28" s="3">
+        <v>22</v>
+      </c>
+      <c r="G28" s="3">
+        <v>23</v>
+      </c>
+      <c r="H28" s="3">
+        <v>24</v>
+      </c>
+      <c r="I28" s="3">
+        <v>25</v>
+      </c>
+      <c r="J28" s="3">
+        <v>26</v>
+      </c>
+      <c r="K28" s="3">
+        <v>27</v>
+      </c>
+      <c r="L28" s="3">
+        <v>28</v>
+      </c>
+      <c r="M28" s="3">
+        <v>29</v>
+      </c>
+      <c r="N28" s="3">
+        <v>30</v>
+      </c>
+      <c r="O28" s="3">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
+      <c r="A29" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="4">
+        <v>40040005</v>
+      </c>
+      <c r="D29" s="3">
+        <v>21</v>
+      </c>
+      <c r="E29" s="3">
+        <v>22</v>
+      </c>
+      <c r="F29" s="3">
+        <v>23</v>
+      </c>
+      <c r="G29" s="3">
+        <v>24</v>
+      </c>
+      <c r="H29" s="3">
+        <v>25</v>
+      </c>
+      <c r="I29" s="3">
+        <v>26</v>
+      </c>
+      <c r="J29" s="3">
+        <v>27</v>
+      </c>
+      <c r="K29" s="3">
+        <v>28</v>
+      </c>
+      <c r="L29" s="3">
+        <v>29</v>
+      </c>
+      <c r="M29" s="3">
+        <v>30</v>
+      </c>
+      <c r="N29" s="3">
+        <v>31</v>
+      </c>
+      <c r="O29" s="3">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="A30" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="4">
+        <v>40041002</v>
+      </c>
+      <c r="D30" s="3">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3">
+        <v>23</v>
+      </c>
+      <c r="F30" s="3">
+        <v>24</v>
+      </c>
+      <c r="G30" s="3">
+        <v>25</v>
+      </c>
+      <c r="H30" s="3">
+        <v>26</v>
+      </c>
+      <c r="I30" s="3">
+        <v>27</v>
+      </c>
+      <c r="J30" s="3">
+        <v>28</v>
+      </c>
+      <c r="K30" s="3">
+        <v>29</v>
+      </c>
+      <c r="L30" s="3">
+        <v>30</v>
+      </c>
+      <c r="M30" s="3">
+        <v>31</v>
+      </c>
+      <c r="N30" s="3">
+        <v>32</v>
+      </c>
+      <c r="O30" s="3">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
+      <c r="A31" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="4">
+        <v>40041000</v>
+      </c>
+      <c r="D31" s="3">
+        <v>23</v>
+      </c>
+      <c r="E31" s="3">
+        <v>24</v>
+      </c>
+      <c r="F31" s="3">
+        <v>25</v>
+      </c>
+      <c r="G31" s="3">
+        <v>26</v>
+      </c>
+      <c r="H31" s="3">
+        <v>27</v>
+      </c>
+      <c r="I31" s="3">
+        <v>28</v>
+      </c>
+      <c r="J31" s="3">
+        <v>29</v>
+      </c>
+      <c r="K31" s="3">
+        <v>30</v>
+      </c>
+      <c r="L31" s="3">
+        <v>31</v>
+      </c>
+      <c r="M31" s="3">
+        <v>32</v>
+      </c>
+      <c r="N31" s="3">
+        <v>33</v>
+      </c>
+      <c r="O31" s="3">
+        <v>34</v>
+      </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
+      <c r="A32" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="4">
+        <v>40043000</v>
+      </c>
+      <c r="D32" s="3">
+        <v>24</v>
+      </c>
+      <c r="E32" s="3">
+        <v>25</v>
+      </c>
+      <c r="F32" s="3">
+        <v>26</v>
+      </c>
+      <c r="G32" s="3">
+        <v>27</v>
+      </c>
+      <c r="H32" s="3">
+        <v>28</v>
+      </c>
+      <c r="I32" s="3">
+        <v>29</v>
+      </c>
+      <c r="J32" s="3">
+        <v>30</v>
+      </c>
+      <c r="K32" s="3">
+        <v>31</v>
+      </c>
+      <c r="L32" s="3">
+        <v>32</v>
+      </c>
+      <c r="M32" s="3">
+        <v>33</v>
+      </c>
+      <c r="N32" s="3">
+        <v>34</v>
+      </c>
+      <c r="O32" s="3">
+        <v>35</v>
+      </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
+      <c r="A33" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="4">
+        <v>40043006</v>
+      </c>
+      <c r="D33" s="3">
+        <v>25</v>
+      </c>
+      <c r="E33" s="3">
+        <v>26</v>
+      </c>
+      <c r="F33" s="3">
+        <v>27</v>
+      </c>
+      <c r="G33" s="3">
+        <v>28</v>
+      </c>
+      <c r="H33" s="3">
+        <v>29</v>
+      </c>
+      <c r="I33" s="3">
+        <v>30</v>
+      </c>
+      <c r="J33" s="3">
+        <v>31</v>
+      </c>
+      <c r="K33" s="3">
+        <v>32</v>
+      </c>
+      <c r="L33" s="3">
+        <v>33</v>
+      </c>
+      <c r="M33" s="3">
+        <v>34</v>
+      </c>
+      <c r="N33" s="3">
+        <v>35</v>
+      </c>
+      <c r="O33" s="3">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>

</xml_diff>